<commit_message>
trying delta s2tcompare auto
</commit_message>
<xml_diff>
--- a/datf_core/test/s2t/s2t_34_delta_parquet_auto.xlsx
+++ b/datf_core/test/s2t/s2t_34_delta_parquet_auto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\DATF_Other\Databricks\QE_ATF\datf_core\test\s2t\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65D5E0E-687C-4465-888B-EAE85EC81691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992E45A4-F31E-4BB8-8126-0892AACF1139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{60D25328-0517-4E51-B966-9D3337769260}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="130">
   <si>
     <t>mappingname</t>
   </si>
@@ -326,31 +326,109 @@
     <t>delta</t>
   </si>
   <si>
-    <t>VENDOR</t>
-  </si>
-  <si>
-    <t>ADF_RUN_ID</t>
-  </si>
-  <si>
-    <t>ADF_JOB_ID</t>
-  </si>
-  <si>
     <t>test/data/source</t>
   </si>
   <si>
-    <t>DATETO</t>
-  </si>
-  <si>
-    <t>DATEFROM</t>
-  </si>
-  <si>
-    <t>TXTMD</t>
-  </si>
-  <si>
-    <t>fdp_dev_01.psas_fdp_usp_bronze.t_vendor</t>
-  </si>
-  <si>
-    <t>FDP_source_file</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>BIRTHDATE</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>DEATHDATE</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>DRIVERS</t>
+  </si>
+  <si>
+    <t>PASSPORT</t>
+  </si>
+  <si>
+    <t>PREFIX</t>
+  </si>
+  <si>
+    <t>FIRST</t>
+  </si>
+  <si>
+    <t>LAST</t>
+  </si>
+  <si>
+    <t>SUFFIX</t>
+  </si>
+  <si>
+    <t>MAIDEN</t>
+  </si>
+  <si>
+    <t>MARITAL</t>
+  </si>
+  <si>
+    <t>RACE</t>
+  </si>
+  <si>
+    <t>ETHNICITY</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>BIRTHPLACE</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>COUNTY</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>LAT</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>LON</t>
+  </si>
+  <si>
+    <t>HEALTHCARE_EXPENSES</t>
+  </si>
+  <si>
+    <t>HEALTHCARE_COVERAGE</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>targetdata</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Id_New</t>
+  </si>
+  <si>
+    <t>patients_source_parquet</t>
+  </si>
+  <si>
+    <t>delta_target</t>
+  </si>
+  <si>
+    <t>dbfs:/user/hive/warehouse/healthcare.db</t>
   </si>
 </sst>
 </file>
@@ -788,7 +866,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +944,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -874,7 +952,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -949,14 +1027,16 @@
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1151,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F175362-E919-4E0B-BAAB-8F57DA09A5DB}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,7 +1303,7 @@
         <v>65</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
@@ -1243,13 +1323,13 @@
         <v>65</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D3" s="5">
         <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1260,13 +1340,13 @@
         <v>65</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" s="5">
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1277,10 +1357,10 @@
         <v>65</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>66</v>
@@ -1294,10 +1374,10 @@
         <v>65</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D6" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>66</v>
@@ -1311,10 +1391,10 @@
         <v>65</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D7" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>66</v>
@@ -1322,36 +1402,33 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D8" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D9" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>66</v>
@@ -1359,16 +1436,16 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D10" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>66</v>
@@ -1376,16 +1453,16 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D11" s="5">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>66</v>
@@ -1393,16 +1470,16 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="D12" s="5">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>66</v>
@@ -1410,19 +1487,668 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="D13" s="5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="5">
+        <v>13</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="5">
+        <v>14</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="5">
+        <v>15</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="5">
+        <v>16</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="5">
+        <v>17</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="5">
+        <v>18</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="5">
+        <v>19</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="5">
+        <v>20</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="5">
+        <v>21</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="5">
+        <v>22</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="5">
+        <v>23</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="5">
+        <v>24</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="5">
+        <v>25</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="5">
+        <v>3</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="5">
+        <v>4</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="5">
+        <v>5</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="5">
+        <v>6</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="5">
+        <v>7</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" s="5">
+        <v>8</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="5">
+        <v>9</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="5">
+        <v>10</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="5">
+        <v>11</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="5">
+        <v>12</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="5">
+        <v>13</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="5">
+        <v>14</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="5">
+        <v>15</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="5">
+        <v>16</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="5">
+        <v>17</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="5">
+        <v>18</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D45" s="5">
+        <v>19</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="5">
+        <v>20</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D47" s="5">
+        <v>21</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D48" s="5">
+        <v>22</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="5">
+        <v>23</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" s="5">
+        <v>24</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51" s="5">
+        <v>25</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1440,7 +2166,7 @@
   <dimension ref="A1:M125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,7 +2234,7 @@
         <v>69</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>64</v>
@@ -1517,7 +2243,7 @@
         <v>65</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>83</v>
@@ -1531,7 +2257,7 @@
         <v>69</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>64</v>
@@ -1540,7 +2266,7 @@
         <v>65</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>83</v>
@@ -1554,7 +2280,7 @@
         <v>69</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>64</v>
@@ -1563,7 +2289,7 @@
         <v>65</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>83</v>
@@ -1577,7 +2303,7 @@
         <v>69</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>64</v>
@@ -1586,7 +2312,7 @@
         <v>65</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>83</v>
@@ -1600,7 +2326,7 @@
         <v>69</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>64</v>
@@ -1609,7 +2335,7 @@
         <v>65</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>83</v>
@@ -1623,7 +2349,7 @@
         <v>69</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>64</v>
@@ -1632,9 +2358,446 @@
         <v>65</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1648,10 +2811,10 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{CBF7BB24-3FE4-4A33-AB7A-E3A25EA1C96E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A27:A1048576" xr:uid="{CBF7BB24-3FE4-4A33-AB7A-E3A25EA1C96E}">
       <formula1>"stage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{C1285BA5-A59F-477D-88E5-0DBA94A623F7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D27:D1048576" xr:uid="{C1285BA5-A59F-477D-88E5-0DBA94A623F7}">
       <formula1>"source"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{37AD8DBC-7F2B-40F6-A3CC-4C237BC4137B}">
@@ -1670,7 +2833,7 @@
   <dimension ref="A1:P154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,13 +2907,27 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="A2" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -1762,13 +2939,27 @@
       <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="A3" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -1780,13 +2971,27 @@
       <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="A4" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -1798,13 +3003,27 @@
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="A5" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -1816,13 +3035,27 @@
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="A6" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -1834,13 +3067,27 @@
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="A7" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -1852,13 +3099,27 @@
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="A8" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -1870,13 +3131,27 @@
       <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="A9" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -1888,13 +3163,27 @@
       <c r="P9" s="5"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="A10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -1906,13 +3195,27 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="A11" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1924,13 +3227,27 @@
       <c r="P11" s="5"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="A12" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -1942,13 +3259,27 @@
       <c r="P12" s="5"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="A13" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1960,13 +3291,27 @@
       <c r="P13" s="5"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="A14" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1978,13 +3323,27 @@
       <c r="P14" s="5"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="A15" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1996,13 +3355,27 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="A16" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -2014,13 +3387,27 @@
       <c r="P16" s="5"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="A17" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -2032,13 +3419,27 @@
       <c r="P17" s="5"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="A18" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -2050,13 +3451,27 @@
       <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -2068,13 +3483,27 @@
       <c r="P19" s="5"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="A20" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -2086,13 +3515,27 @@
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="A21" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -2104,13 +3547,27 @@
       <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="A22" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -2122,13 +3579,27 @@
       <c r="P22" s="5"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="A23" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -2140,13 +3611,27 @@
       <c r="P23" s="5"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="A24" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -2158,13 +3643,27 @@
       <c r="P24" s="5"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="A25" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -2176,13 +3675,27 @@
       <c r="P25" s="5"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="A26" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -4471,10 +5984,10 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{E014C82D-A48E-4F23-A792-D29AD91E1240}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A27:A1048576" xr:uid="{E014C82D-A48E-4F23-A792-D29AD91E1240}">
       <formula1>"target"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{09455547-24CF-466D-A644-08FBDC55E54D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D27:D1048576" xr:uid="{09455547-24CF-466D-A644-08FBDC55E54D}">
       <formula1>"stage,source"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P1048576" xr:uid="{B4533C99-D538-4EFF-B76A-7A990E88FE9B}">

</xml_diff>

<commit_message>
fixing the mapping sheet
</commit_message>
<xml_diff>
--- a/datf_core/test/s2t/s2t_34_delta_parquet_auto.xlsx
+++ b/datf_core/test/s2t/s2t_34_delta_parquet_auto.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\DATF_Other\Databricks\QE_ATF\datf_core\test\s2t\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C2C7BD-3D87-48F0-80E0-801B03E84B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BACE5F-0340-419B-802A-AA521071632A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{60D25328-0517-4E51-B966-9D3337769260}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{60D25328-0517-4E51-B966-9D3337769260}"/>
   </bookViews>
   <sheets>
     <sheet name="MappingConfiguration" sheetId="1" r:id="rId1"/>
     <sheet name="Schema" sheetId="2" r:id="rId2"/>
-    <sheet name="StageMapping" sheetId="3" r:id="rId3"/>
-    <sheet name="TargetMapping" sheetId="4" r:id="rId4"/>
+    <sheet name="TargetMapping" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="130">
   <si>
     <t>mappingname</t>
   </si>
@@ -308,9 +307,6 @@
     <t>landing_layer</t>
   </si>
   <si>
-    <t>aws-s3</t>
-  </si>
-  <si>
     <t>parquet</t>
   </si>
   <si>
@@ -329,9 +325,6 @@
     <t>test/data/source</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>BIRTHDATE</t>
   </si>
   <si>
@@ -429,6 +422,12 @@
   </si>
   <si>
     <t>dbfs:/user/hive/warehouse/healthcare.db</t>
+  </si>
+  <si>
+    <t>databricks</t>
+  </si>
+  <si>
+    <t>integer</t>
   </si>
 </sst>
 </file>
@@ -510,7 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -530,9 +529,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -865,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E28631E-9A8B-4B40-8EC8-AD01C3B31856}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +916,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -928,7 +924,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -936,7 +932,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -944,7 +940,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -952,7 +948,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -990,7 +986,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -998,7 +994,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1006,7 +1002,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1014,7 +1010,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1028,7 +1024,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1036,7 +1032,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1073,77 +1069,89 @@
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" s="2"/>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="2"/>
     </row>
     <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="2"/>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B41" s="2"/>
     </row>
@@ -1209,20 +1217,20 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9 B20" xr:uid="{17102121-B8C6-4480-9AF2-64013E9BC832}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9 B20 B32" xr:uid="{17102121-B8C6-4480-9AF2-64013E9BC832}">
       <formula1>"avro,json,parquet,delimitedfile,delta,table"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{3E7D930E-245E-4CA4-A308-BADDF7C7F304}">
-      <formula1>"aws-s3,redshift,oracle"</formula1>
+      <formula1>"aws-s3,redshift,oracle,databricks"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42:B44 B46 B37 B12 B24 B48" xr:uid="{BFE88CB4-E2D3-429E-9E37-28340811242C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42:B44 B46 B36 B12 B24 B48" xr:uid="{BFE88CB4-E2D3-429E-9E37-28340811242C}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47" xr:uid="{68E42079-4681-420E-B4F0-F089CD1AE25F}">
       <formula1>"insert_only,insert_update"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19" xr:uid="{E8B6213B-2975-4740-AC52-AAD0EC2882DD}">
-      <formula1>"aws-s3,redshift,oracle,mysql"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19 B31" xr:uid="{E8B6213B-2975-4740-AC52-AAD0EC2882DD}">
+      <formula1>"aws-s3,redshift,oracle,mysql,databricks"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1231,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F175362-E919-4E0B-BAAB-8F57DA09A5DB}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,7 +1311,7 @@
         <v>65</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
@@ -1323,13 +1331,13 @@
         <v>65</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D3" s="5">
         <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1340,13 +1348,13 @@
         <v>65</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D4" s="5">
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1357,7 +1365,7 @@
         <v>65</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D5" s="5">
         <v>4</v>
@@ -1374,7 +1382,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D6" s="5">
         <v>5</v>
@@ -1391,7 +1399,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D7" s="5">
         <v>6</v>
@@ -1408,7 +1416,7 @@
         <v>65</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D8" s="5">
         <v>7</v>
@@ -1425,7 +1433,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D9" s="5">
         <v>8</v>
@@ -1442,7 +1450,7 @@
         <v>65</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D10" s="5">
         <v>9</v>
@@ -1459,7 +1467,7 @@
         <v>65</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D11" s="5">
         <v>10</v>
@@ -1476,7 +1484,7 @@
         <v>65</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D12" s="5">
         <v>11</v>
@@ -1493,7 +1501,7 @@
         <v>65</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D13" s="5">
         <v>12</v>
@@ -1510,7 +1518,7 @@
         <v>65</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D14" s="5">
         <v>13</v>
@@ -1527,7 +1535,7 @@
         <v>65</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D15" s="5">
         <v>14</v>
@@ -1544,7 +1552,7 @@
         <v>65</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D16" s="5">
         <v>15</v>
@@ -1561,7 +1569,7 @@
         <v>65</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D17" s="5">
         <v>16</v>
@@ -1578,7 +1586,7 @@
         <v>65</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D18" s="5">
         <v>17</v>
@@ -1595,7 +1603,7 @@
         <v>65</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D19" s="5">
         <v>18</v>
@@ -1612,7 +1620,7 @@
         <v>65</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D20" s="5">
         <v>19</v>
@@ -1629,7 +1637,7 @@
         <v>65</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D21" s="5">
         <v>20</v>
@@ -1646,7 +1654,7 @@
         <v>65</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D22" s="5">
         <v>21</v>
@@ -1663,13 +1671,13 @@
         <v>65</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D23" s="5">
         <v>22</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1680,13 +1688,13 @@
         <v>65</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D24" s="5">
         <v>23</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1697,13 +1705,13 @@
         <v>65</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D25" s="5">
         <v>24</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1714,13 +1722,13 @@
         <v>65</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D26" s="5">
         <v>25</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1731,7 +1739,7 @@
         <v>69</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D27" s="5">
         <v>1</v>
@@ -1751,13 +1759,13 @@
         <v>69</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D28" s="5">
         <v>2</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1768,13 +1776,13 @@
         <v>69</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D29" s="5">
         <v>3</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1785,7 +1793,7 @@
         <v>69</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D30" s="5">
         <v>4</v>
@@ -1802,7 +1810,7 @@
         <v>69</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D31" s="5">
         <v>5</v>
@@ -1819,7 +1827,7 @@
         <v>69</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D32" s="5">
         <v>6</v>
@@ -1836,7 +1844,7 @@
         <v>69</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D33" s="5">
         <v>7</v>
@@ -1853,7 +1861,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D34" s="5">
         <v>8</v>
@@ -1870,7 +1878,7 @@
         <v>69</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D35" s="5">
         <v>9</v>
@@ -1887,7 +1895,7 @@
         <v>69</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D36" s="5">
         <v>10</v>
@@ -1904,7 +1912,7 @@
         <v>69</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D37" s="5">
         <v>11</v>
@@ -1921,7 +1929,7 @@
         <v>69</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D38" s="5">
         <v>12</v>
@@ -1938,7 +1946,7 @@
         <v>69</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D39" s="5">
         <v>13</v>
@@ -1955,7 +1963,7 @@
         <v>69</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D40" s="5">
         <v>14</v>
@@ -1972,7 +1980,7 @@
         <v>69</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D41" s="5">
         <v>15</v>
@@ -1989,7 +1997,7 @@
         <v>69</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D42" s="5">
         <v>16</v>
@@ -2006,7 +2014,7 @@
         <v>69</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D43" s="5">
         <v>17</v>
@@ -2023,7 +2031,7 @@
         <v>69</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D44" s="5">
         <v>18</v>
@@ -2040,7 +2048,7 @@
         <v>69</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D45" s="5">
         <v>19</v>
@@ -2057,7 +2065,7 @@
         <v>69</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D46" s="5">
         <v>20</v>
@@ -2074,13 +2082,13 @@
         <v>69</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D47" s="5">
         <v>21</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>66</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2091,16 +2099,16 @@
         <v>69</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D48" s="5">
         <v>22</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>68</v>
       </c>
@@ -2108,16 +2116,16 @@
         <v>69</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D49" s="5">
         <v>23</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>68</v>
       </c>
@@ -2125,16 +2133,16 @@
         <v>69</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D50" s="5">
         <v>24</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>68</v>
       </c>
@@ -2142,13 +2150,441 @@
         <v>69</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D51" s="5">
         <v>25</v>
       </c>
       <c r="E51" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D52" s="5">
+        <v>1</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53" s="5">
+        <v>2</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" s="5">
+        <v>3</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="5">
+        <v>4</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" s="5">
+        <v>5</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57" s="5">
+        <v>6</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" s="5">
+        <v>7</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D59" s="5">
+        <v>8</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D60" s="5">
+        <v>9</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D61" s="5">
+        <v>10</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D62" s="5">
+        <v>11</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D63" s="5">
+        <v>12</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D64" s="5">
+        <v>13</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D65" s="5">
+        <v>14</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D66" s="5">
+        <v>15</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" s="5">
+        <v>16</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D68" s="5">
+        <v>17</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D69" s="5">
+        <v>18</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D70" s="5">
+        <v>19</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D71" s="5">
+        <v>20</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D72" s="5">
+        <v>21</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D73" s="5">
+        <v>22</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D74" s="5">
+        <v>23</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C75" s="5" t="s">
         <v>119</v>
+      </c>
+      <c r="D75" s="5">
+        <v>24</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D76" s="5">
+        <v>25</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2162,698 +2598,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2474D01D-161E-4691-B370-B8E9C603A9D5}">
-  <dimension ref="A1:M125"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1B550D-10B7-4DED-8B4E-101137D895D9}">
+  <dimension ref="A1:P154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="61.140625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="32.42578125" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="123" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I123" s="9"/>
-      <c r="J123" s="9"/>
-    </row>
-    <row r="125" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I125" s="9"/>
-      <c r="J125" s="9"/>
-    </row>
-  </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A27:A1048576" xr:uid="{CBF7BB24-3FE4-4A33-AB7A-E3A25EA1C96E}">
-      <formula1>"stage"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D27:D1048576" xr:uid="{C1285BA5-A59F-477D-88E5-0DBA94A623F7}">
-      <formula1>"source"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{37AD8DBC-7F2B-40F6-A3CC-4C237BC4137B}">
-      <formula1>"Y,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{4BD702AC-109D-4CA1-AAEA-CDEC3A5F7BEA}">
-      <formula1>"directmapped,derived"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1B550D-10B7-4DED-8B4E-101137D895D9}">
-  <dimension ref="A1:P154"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="56.85546875" style="10" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" style="10" customWidth="1"/>
-    <col min="11" max="11" width="27" style="10" customWidth="1"/>
-    <col min="12" max="12" width="22.5703125" style="10" customWidth="1"/>
-    <col min="13" max="13" width="22.7109375" style="10" customWidth="1"/>
-    <col min="14" max="14" width="25.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="56.85546875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="37.85546875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="27" style="9" customWidth="1"/>
+    <col min="12" max="12" width="22.5703125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" style="9" customWidth="1"/>
+    <col min="14" max="14" width="25.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.5703125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -2908,13 +2677,13 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>64</v>
@@ -2923,7 +2692,7 @@
         <v>65</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>83</v>
@@ -2940,13 +2709,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>64</v>
@@ -2955,7 +2724,7 @@
         <v>65</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>83</v>
@@ -2972,13 +2741,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>64</v>
@@ -2987,7 +2756,7 @@
         <v>65</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>83</v>
@@ -3004,13 +2773,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>64</v>
@@ -3019,7 +2788,7 @@
         <v>65</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>83</v>
@@ -3036,13 +2805,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>64</v>
@@ -3051,7 +2820,7 @@
         <v>65</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>83</v>
@@ -3068,13 +2837,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>64</v>
@@ -3083,7 +2852,7 @@
         <v>65</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>83</v>
@@ -3100,13 +2869,13 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>64</v>
@@ -3115,7 +2884,7 @@
         <v>65</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>83</v>
@@ -3132,13 +2901,13 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>64</v>
@@ -3147,7 +2916,7 @@
         <v>65</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>83</v>
@@ -3164,13 +2933,13 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>64</v>
@@ -3179,7 +2948,7 @@
         <v>65</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>83</v>
@@ -3196,13 +2965,13 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>64</v>
@@ -3211,7 +2980,7 @@
         <v>65</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>83</v>
@@ -3228,13 +2997,13 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>64</v>
@@ -3243,7 +3012,7 @@
         <v>65</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>83</v>
@@ -3260,13 +3029,13 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>64</v>
@@ -3275,7 +3044,7 @@
         <v>65</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>83</v>
@@ -3292,13 +3061,13 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>64</v>
@@ -3307,7 +3076,7 @@
         <v>65</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>83</v>
@@ -3324,13 +3093,13 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>64</v>
@@ -3339,7 +3108,7 @@
         <v>65</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>83</v>
@@ -3356,13 +3125,13 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>64</v>
@@ -3371,7 +3140,7 @@
         <v>65</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>83</v>
@@ -3388,13 +3157,13 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>64</v>
@@ -3403,7 +3172,7 @@
         <v>65</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>83</v>
@@ -3420,13 +3189,13 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>64</v>
@@ -3435,7 +3204,7 @@
         <v>65</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>83</v>
@@ -3452,13 +3221,13 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>64</v>
@@ -3467,7 +3236,7 @@
         <v>65</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>83</v>
@@ -3484,13 +3253,13 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>64</v>
@@ -3499,7 +3268,7 @@
         <v>65</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>83</v>
@@ -3516,13 +3285,13 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>64</v>
@@ -3531,7 +3300,7 @@
         <v>65</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>83</v>
@@ -3548,13 +3317,13 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>64</v>
@@ -3563,7 +3332,7 @@
         <v>65</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>83</v>
@@ -3580,13 +3349,13 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>64</v>
@@ -3595,7 +3364,7 @@
         <v>65</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>83</v>
@@ -3612,13 +3381,13 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>64</v>
@@ -3627,7 +3396,7 @@
         <v>65</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>83</v>
@@ -3644,13 +3413,13 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>64</v>
@@ -3659,7 +3428,7 @@
         <v>65</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>83</v>
@@ -3676,13 +3445,13 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>64</v>
@@ -3691,7 +3460,7 @@
         <v>65</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>83</v>
@@ -5768,7 +5537,7 @@
       <c r="G141" s="5"/>
       <c r="H141" s="5"/>
       <c r="I141" s="5"/>
-      <c r="J141" s="8"/>
+      <c r="J141" s="7"/>
       <c r="K141" s="5"/>
       <c r="L141" s="5"/>
       <c r="M141" s="5"/>
@@ -5785,7 +5554,7 @@
       <c r="F142" s="5"/>
       <c r="G142" s="5"/>
       <c r="H142" s="5"/>
-      <c r="J142" s="9"/>
+      <c r="J142" s="8"/>
       <c r="K142" s="5"/>
       <c r="L142" s="5"/>
       <c r="M142" s="5"/>
@@ -5803,7 +5572,7 @@
       <c r="G143" s="5"/>
       <c r="H143" s="5"/>
       <c r="I143" s="5"/>
-      <c r="J143" s="8"/>
+      <c r="J143" s="7"/>
       <c r="K143" s="5"/>
       <c r="L143" s="5"/>
       <c r="M143" s="5"/>
@@ -5821,7 +5590,7 @@
       <c r="G144" s="5"/>
       <c r="H144" s="5"/>
       <c r="I144" s="5"/>
-      <c r="J144" s="9"/>
+      <c r="J144" s="8"/>
       <c r="K144" s="5"/>
       <c r="L144" s="5"/>
       <c r="M144" s="5"/>
@@ -5946,7 +5715,7 @@
       <c r="F152" s="5"/>
       <c r="G152" s="5"/>
       <c r="H152" s="5"/>
-      <c r="I152" s="11"/>
+      <c r="I152" s="10"/>
       <c r="K152" s="5"/>
       <c r="N152" s="5"/>
       <c r="O152" s="5"/>
@@ -5976,7 +5745,7 @@
       <c r="F154" s="5"/>
       <c r="G154" s="5"/>
       <c r="H154" s="5"/>
-      <c r="I154" s="11"/>
+      <c r="I154" s="10"/>
       <c r="K154" s="5"/>
       <c r="N154" s="5"/>
       <c r="O154" s="5"/>

</xml_diff>